<commit_message>
Arquivos prontos para entrega
</commit_message>
<xml_diff>
--- a/17- Análise de Eventos para cada Cenário .xlsx
+++ b/17- Análise de Eventos para cada Cenário .xlsx
@@ -1,40 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alisson A. Alves\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alisson A. Alves\Desktop\Faculdade\2º Semestre\Engenharia de Software\Nossos_artefatos\Engenharia_de_software-TPD_Grafica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8DAFB90-789F-4671-A3EB-F434ED936326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F14351B-631B-4F3C-B77B-AF50D70C75A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
   <si>
     <t>Externo</t>
   </si>
@@ -69,9 +60,6 @@
     <t>Extemporâneo</t>
   </si>
   <si>
-    <t>Receber solicitação de serviços</t>
-  </si>
-  <si>
     <t>FB</t>
   </si>
   <si>
@@ -111,45 +99,57 @@
     <t>x(5)</t>
   </si>
   <si>
-    <t>Comprar
-produtos
-prontos</t>
-  </si>
-  <si>
     <t>Cliente realiza pedido</t>
-  </si>
-  <si>
-    <t>Retirar
-produtos</t>
-  </si>
-  <si>
-    <t>Cliente solicita
-retirada de produto</t>
-  </si>
-  <si>
-    <t>Fechar
-parceria</t>
   </si>
   <si>
     <t>Empresa realiza pedido
 de parceria</t>
-  </si>
-  <si>
-    <t>Receber pelos
-serviços 
-realizados</t>
   </si>
   <si>
     <t>Parceiro solicita
 pagamento pelos 
 serviços prestados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliente retorna sobre valor (cartão) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliente retorna sobre valor (dinheiro) </t>
+  </si>
+  <si>
+    <t>Atendente finaliza pedido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atendente entrega produto de encomenda </t>
+  </si>
+  <si>
+    <t>Cliente solicita
+retirada de produto de encomenda</t>
+  </si>
+  <si>
+    <t>Tratar solicitação de serviços</t>
+  </si>
+  <si>
+    <t>Vender produtos prontos</t>
+  </si>
+  <si>
+    <t>Tratar saída de produtos</t>
+  </si>
+  <si>
+    <t>Tratar parceria de negócio</t>
+  </si>
+  <si>
+    <t>Tratar pagamento de serviços realizados</t>
+  </si>
+  <si>
+    <t>Atendente finaliza retirada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -342,11 +342,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -400,9 +435,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -432,6 +464,36 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,13 +781,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K35"/>
+  <dimension ref="B2:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
@@ -735,23 +797,23 @@
     <col min="6" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="2:11" ht="30" customHeight="1">
+    <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -781,39 +843,39 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="30" customHeight="1">
-      <c r="B4" s="25" t="s">
+    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="2:11" ht="41.25" customHeight="1">
-      <c r="B5" s="26"/>
-      <c r="C5" s="23"/>
+    <row r="5" spans="2:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="25"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="5">
         <v>2</v>
       </c>
       <c r="E5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="9"/>
@@ -821,37 +883,37 @@
       <c r="J5" s="10"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="2:11" ht="27.75" customHeight="1">
-      <c r="B6" s="26"/>
-      <c r="C6" s="24"/>
+    <row r="6" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="25"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="5">
         <v>3</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="2:11" ht="38.25" customHeight="1">
-      <c r="B7" s="26"/>
-      <c r="C7" s="22" t="s">
-        <v>19</v>
+    <row r="7" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="25"/>
+      <c r="C7" s="21" t="s">
+        <v>18</v>
       </c>
       <c r="D7" s="5">
         <v>4</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="9"/>
@@ -859,53 +921,53 @@
       <c r="J7" s="10"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="2:11" ht="30" customHeight="1">
-      <c r="B8" s="26"/>
-      <c r="C8" s="23"/>
+    <row r="8" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="25"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="5">
         <v>5</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="2:11" ht="38.25" customHeight="1">
-      <c r="B9" s="26"/>
-      <c r="C9" s="23"/>
+    <row r="9" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="25"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="5">
         <v>6</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="9"/>
       <c r="I9" s="10"/>
       <c r="J9" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="2:11">
-      <c r="B10" s="27"/>
-      <c r="C10" s="24"/>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="26"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="5">
         <v>7</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
@@ -913,25 +975,25 @@
       <c r="J10" s="10"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="2:11" ht="24.75" customHeight="1"/>
-    <row r="12" spans="2:11" ht="24.75" customHeight="1"/>
-    <row r="13" spans="2:11" ht="24.75" customHeight="1">
+    <row r="11" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20" t="s">
+      <c r="G13" s="19"/>
+      <c r="H13" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="2:11" ht="24.75" customHeight="1">
+    <row r="14" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>2</v>
       </c>
@@ -961,39 +1023,39 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="24.75" customHeight="1">
-      <c r="B15" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>12</v>
+    <row r="15" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>11</v>
       </c>
       <c r="D15" s="15">
         <v>1</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="2:11" ht="45" customHeight="1">
-      <c r="B16" s="21"/>
+    <row r="16" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="20"/>
       <c r="C16" s="29"/>
       <c r="D16" s="15">
         <v>2</v>
       </c>
       <c r="E16" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="9"/>
@@ -1001,19 +1063,17 @@
       <c r="J16" s="9"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="2:11" ht="45" customHeight="1">
-      <c r="B17" s="21"/>
-      <c r="C17" s="16" t="s">
-        <v>19</v>
-      </c>
+    <row r="17" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="20"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="15">
         <v>3</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="9"/>
@@ -1021,236 +1081,294 @@
       <c r="J17" s="9"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="2:11" ht="24.75" customHeight="1"/>
-    <row r="19" spans="2:11" ht="24.75" customHeight="1"/>
-    <row r="20" spans="2:11" ht="24.75" customHeight="1">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="20" t="s">
+    <row r="18" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="20"/>
+      <c r="C18" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="15">
+        <v>4</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20" t="s">
+      <c r="G21" s="19"/>
+      <c r="H21" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="2:11" ht="24.75" customHeight="1">
-      <c r="B21" s="11" t="s">
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="11" t="s">
+      <c r="C22" s="13"/>
+      <c r="D22" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="I22" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="J22" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="K22" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="45" customHeight="1">
-      <c r="B22" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="14">
+    <row r="23" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="35">
         <v>1</v>
       </c>
-      <c r="E22" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="7"/>
-    </row>
-    <row r="23" spans="2:11" ht="24.75" customHeight="1"/>
-    <row r="24" spans="2:11" ht="24.75" customHeight="1"/>
-    <row r="25" spans="2:11" ht="24.75" customHeight="1">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="20" t="s">
+      <c r="E23" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="33"/>
+    </row>
+    <row r="24" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="38"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="36">
+        <v>2</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="33"/>
+    </row>
+    <row r="25" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="38"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="36">
+        <v>3</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20" t="s">
+      <c r="G28" s="19"/>
+      <c r="H28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="2:11" ht="24.75" customHeight="1">
-      <c r="B26" s="11" t="s">
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="11" t="s">
+      <c r="C29" s="13"/>
+      <c r="D29" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E29" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F29" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G29" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H29" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="I29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="J29" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K26" s="11" t="s">
+      <c r="K29" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="30" customHeight="1">
-      <c r="B27" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="17">
+    <row r="30" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="17">
         <v>1</v>
       </c>
-      <c r="E27" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="7"/>
-    </row>
-    <row r="28" spans="2:11" ht="24.75" customHeight="1"/>
-    <row r="29" spans="2:11" ht="24.75" customHeight="1"/>
-    <row r="30" spans="2:11" ht="24.75" customHeight="1">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="20" t="s">
+      <c r="E30" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20" t="s">
+      <c r="G33" s="19"/>
+      <c r="H33" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="2:11" ht="24.75" customHeight="1">
-      <c r="B31" s="11" t="s">
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="11" t="s">
+      <c r="C34" s="13"/>
+      <c r="D34" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E34" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F34" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G34" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H34" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="I34" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J31" s="12" t="s">
+      <c r="J34" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K31" s="11" t="s">
+      <c r="K34" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="45" customHeight="1">
-      <c r="B32" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="14">
+    <row r="35" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="14">
         <v>1</v>
       </c>
-      <c r="E32" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" s="9"/>
-      <c r="K32" s="7"/>
-    </row>
-    <row r="33" ht="24.75" customHeight="1"/>
-    <row r="34" ht="24.75" customHeight="1"/>
-    <row r="35" ht="24.75" customHeight="1"/>
+      <c r="E35" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" s="9"/>
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="B4:B10"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C15:C17"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:J13"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:J21"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>